<commit_message>
~ draft for Problrm 10
</commit_message>
<xml_diff>
--- a/analytics/Problem 10.xlsx
+++ b/analytics/Problem 10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apu/Documents/AndreyPudov/leetcode/analytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4673D15-1E3C-854D-B29E-DAB78B9901CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC4F560-8D82-4E4F-BA55-EB4FBB1ABB20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7960" yWindow="1260" windowWidth="22540" windowHeight="18720" xr2:uid="{43FAE6EE-22B1-C845-A25C-3534ED84BAA5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="22">
   <si>
     <t>m</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>i*</t>
+  </si>
+  <si>
+    <t>.*c</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>bbbba</t>
   </si>
 </sst>
 </file>
@@ -521,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0239EB-22C6-AB49-8F5F-702F95656B93}">
-  <dimension ref="A1:AA51"/>
+  <dimension ref="A1:AA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1129,8 +1138,11 @@
       <c r="A48" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C48" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>7</v>
       </c>
@@ -1138,12 +1150,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D50" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
@@ -1151,10 +1166,181 @@
         <v>1</v>
       </c>
     </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B54" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="6"/>
+      <c r="M54" s="6"/>
+      <c r="N54" s="6"/>
+      <c r="O54" s="6"/>
+      <c r="P54" s="6"/>
+      <c r="Q54" s="6"/>
+      <c r="R54" s="6"/>
+      <c r="S54" s="6"/>
+      <c r="T54" s="6"/>
+      <c r="U54" s="6"/>
+      <c r="V54" s="6"/>
+      <c r="W54" s="6"/>
+      <c r="X54" s="6"/>
+      <c r="Y54" s="6"/>
+      <c r="Z54" s="6"/>
+      <c r="AA54" s="6"/>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" s="7">
+        <v>1</v>
+      </c>
+      <c r="C56" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B60" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="6"/>
+      <c r="K60" s="6"/>
+      <c r="L60" s="6"/>
+      <c r="M60" s="6"/>
+      <c r="N60" s="6"/>
+      <c r="O60" s="6"/>
+      <c r="P60" s="6"/>
+      <c r="Q60" s="6"/>
+      <c r="R60" s="6"/>
+      <c r="S60" s="6"/>
+      <c r="T60" s="6"/>
+      <c r="U60" s="6"/>
+      <c r="V60" s="6"/>
+      <c r="W60" s="6"/>
+      <c r="X60" s="6"/>
+      <c r="Y60" s="6"/>
+      <c r="Z60" s="6"/>
+      <c r="AA60" s="6"/>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B61" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B66" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="6"/>
+      <c r="K66" s="6"/>
+      <c r="L66" s="6"/>
+      <c r="M66" s="6"/>
+      <c r="N66" s="6"/>
+      <c r="O66" s="6"/>
+      <c r="P66" s="6"/>
+      <c r="Q66" s="6"/>
+      <c r="R66" s="6"/>
+      <c r="S66" s="6"/>
+      <c r="T66" s="6"/>
+      <c r="U66" s="6"/>
+      <c r="V66" s="6"/>
+      <c r="W66" s="6"/>
+      <c r="X66" s="6"/>
+      <c r="Y66" s="6"/>
+      <c r="Z66" s="6"/>
+      <c r="AA66" s="6"/>
+    </row>
+    <row r="67" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B67" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+    </row>
+    <row r="69" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
     <mergeCell ref="B35:AA35"/>
     <mergeCell ref="B45:AA45"/>
+    <mergeCell ref="B54:AA54"/>
+    <mergeCell ref="B60:AA60"/>
+    <mergeCell ref="B66:AA66"/>
     <mergeCell ref="B19:AA19"/>
     <mergeCell ref="B30:AA30"/>
     <mergeCell ref="B1:AA1"/>

</xml_diff>